<commit_message>
better code second test
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Youtube names scrapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,177 +434,249 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>video titles</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Cyber Security In 7 Minutes | What Is Cyber Security: How It Works? | Cyber Security | Simplilearn</t>
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Web Scraping Facebook with Selenium - AUTOMATED BOT</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Cyber Security Full Course for Beginner</t>
+      <c r="A3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Scrape Any Facebook Group's Posts with Selenium &amp; BeautifulSoup (Free, works for private groups!)</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Getting Into Cyber Security: 5 Skills You NEED to Learn</t>
+      <c r="A4" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Web Scraping using Python and Selenium | Scrape Facebook | Part 5 | Data Making | DM | DataMaking</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>TryHackMe - Advent of Cyber - 25 Days to Learn Cyber Security</t>
+      <c r="A5" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>How to SCRAPE DYNAMIC websites with Selenium</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Cybersecurity Expert Answers Hacking Questions From Twitter | Tech Support | WIRED</t>
+      <c r="A6" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Python Webcrape Facebook Marketplace</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Cybersecurity: Crash Course Computer Science #31</t>
+      <c r="A7" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Python Selenium- Facebook Marketplace Webscrape Part2</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>The Five Laws of Cybersecurity | Nick Espinosa | TEDxFondduLac</t>
+      <c r="A8" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Facebook Post Comments Scraper Using Python Selenium</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Cybersecurity Expert Demonstrates How Hackers Easily Gain Access To Sensitive Information</t>
+      <c r="A9" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Top 3 FREE Methods using Email Extractor for FREE Email Marketing email extractor free</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Cybersecurity 101</t>
+      <c r="A10" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Facebook Page Scraping | Scraping B2B Pages For Emails And Phone Numbers In 2021 💲 Scrapebox 👈</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Why Cybersecurity is Important! | Romeo Farinacci | TEDxGrandCanyonUniversity</t>
+      <c r="A11" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Scrape Emails From Facebook Business Pages With Scrapebox : Updated Method For 2020</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Introduction to Cybersecurity</t>
+      <c r="A12" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Scrape Any Website Without Code | Generate Leads | Collect Any Data</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Cyber Security Full Course - Learn Cyber Security In 8 Hours | Cyber Security Training |Simplilearn</t>
+      <c r="A13" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Web Scraping Instagram with Selenium</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Cybersecurity and Cybercrime Bill : l'intervention de Shakeel Mohamed</t>
+      <c r="A14" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Python Selenium Tutorial #1 - Web Scraping, Bots &amp; Testing</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>White House backs Kamala Harris after reports of political dysfunction, tension with Biden</t>
+      <c r="A15" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Beautifulsoup vs Selenium vs Scrapy - Which tool for web scraping in 2021?</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>5 Things I Wish I Knew Before Cyber Security</t>
+      <c r="A16" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>(Python)Get Facebook Page Data using Python Scraping (Selenium)</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Why The U.S. Can't Stop Cyber Attacks</t>
+      <c r="A17" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Python Web Scraping - Should I use Selenium, Beautiful Soup or Scrapy? [2020]</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>How I would learn cybersecurity (if I could start over)</t>
+      <c r="A18" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>How to scrape INFINITE scrolling pages using Python and Selenium (2 Methods)</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>A View from the Front Lines of Cybersecurity</t>
+      <c r="A19" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>👥 Facebook Data Scraping &amp; Legal Deep Dive - Free HAR File Tool to Responsibly Extract Facebook Data</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>How Israel Rules The World Of Cyber Security | VICE on HBO</t>
+      <c r="A20" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>#8 How To Automate Facebook Registration /Login Using Selenium Webdriver-Selenium Python Script</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>An Introduction to Cybersecurity Careers</t>
+      <c r="A21" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Web Scraping EP4: bruteforcing facebook with selenium</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>10 REASONS WHY I LIKE THE CYBERSECURITY FIELD</t>
+      <c r="A22" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>How To Scrape Facebook For 1000's Of Leads For Free. No-Code</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>DON'T GET A CYBERSECURITY DEGREE</t>
+      <c r="A23" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Facebook sues developer | Let's talk about data scraping</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Why Isn’t U.S. Cybersecurity Infrastructure Good Enough?</t>
+      <c r="A24" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>How to Scrape Websites Without Getting Blacklisted or Blocked</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>What does a Cybersecurity Analyst Do? Salaries, Skills &amp; Job Outlook</t>
+      <c r="A25" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>WEB SCRAPING made simple with JAVASCRIPT tutorial</t>
         </is>
       </c>
     </row>

</xml_diff>